<commit_message>
Changes in some scripts
</commit_message>
<xml_diff>
--- a/ControllerCal/Steady states calculation SLOW/SLOW model.xlsx
+++ b/ControllerCal/Steady states calculation SLOW/SLOW model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Optimus-2022\ControllerCal\Steady states calculation SLOW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A13CEC-515C-434B-AF17-5BADCA095936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4EC0E7-042F-46C6-866B-55B23569BD61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54F2F4CB-6433-4C74-BEC1-0D40A83789B0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{54F2F4CB-6433-4C74-BEC1-0D40A83789B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>800000</v>
+        <v>40996</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>14</v>
@@ -692,7 +692,7 @@
       </c>
       <c r="B18">
         <f>B4+B5+(B6/B7^2)</f>
-        <v>3122843312.0000005</v>
+        <v>626462078.41000009</v>
       </c>
     </row>
   </sheetData>

</xml_diff>